<commit_message>
I think its done
</commit_message>
<xml_diff>
--- a/Lab 10/city_locations_test.xlsx
+++ b/Lab 10/city_locations_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\BCIT Work Synced Folder\My Courses\COMP3522 OOP 2\Fall 2019\Week 12\Lecture 1\W12 L1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Norman\PycharmProjects\3522_Assignment_2_A01043914_A00893016\Lab 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C6025A-63D0-487C-B1B6-13C5A0E9ADA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129AB7EA-E845-4EBF-AC8F-FAE3DC7DC4FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25095" yWindow="2280" windowWidth="22815" windowHeight="14850" xr2:uid="{86E8A028-58B2-4029-8ACE-F76B7C3B81F8}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="32295" windowHeight="14955" xr2:uid="{86E8A028-58B2-4029-8ACE-F76B7C3B81F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>